<commit_message>
add func get_str_K1237 to import data from file
</commit_message>
<xml_diff>
--- a/files/tab p2.xlsx
+++ b/files/tab p2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="510" windowWidth="24615" windowHeight="13740"/>
+    <workbookView xWindow="270" yWindow="570" windowWidth="24615" windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="281">
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
   <si>
     <r>
       <rPr>
@@ -22,24 +58,6 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t>2</t>
     </r>
   </si>
@@ -49,134 +67,25 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>6</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>9</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>10</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>11</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>12</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>13</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
+      <t xml:space="preserve">Акролеин </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>(H</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
       <t>2</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">Акролеин </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>(H</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
     <r>
       <rPr>
         <i/>
@@ -184,56 +93,6 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t>C)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Аммиак (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>NH</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>хранение под давлением</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>изотермическое хранение</t>
     </r>
   </si>
   <si>
@@ -1617,150 +1476,6 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>14</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>16</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>17</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>18</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>19</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>21</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>22</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>23</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>26</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>28</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>29</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>30</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t xml:space="preserve">Метилакрилат </t>
     </r>
     <r>
@@ -2079,23 +1794,6 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t xml:space="preserve">Соляная кислота (концентрированная) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>(HCI)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t xml:space="preserve">Триметиламин </t>
     </r>
     <r>
@@ -3217,42 +2915,6 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>31</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>32</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>33</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>34</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t xml:space="preserve">Хлорциан </t>
     </r>
     <r>
@@ -3495,38 +3157,6 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>0,1*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">* * </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">&lt;N </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t>0,04</t>
     </r>
   </si>
@@ -3702,182 +3332,48 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Примечания:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>1. Плотности газообразных АХОВ в графе 3 приведены для атмосферного давления; при давлении в емкости, отличном от атмосфер-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>ного, плотности определяются путем умножения данных графы 3 на значение давления в атмосферах (1 атм = 760 мм рт. ст.).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">2. Значения </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>К</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> в графах 10-14 в числителе приведены для первичного, в знаменателе - для вторичного облака.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>3. В графе 6 численные значения токсодоз, помеченные звездочками, определены ориентировочно по соотношению:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Д=240 КПДКр.з</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, где </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Д</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> - токсодоза, мгмин/л; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>ПДКр.з</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> - ПДК рабочей зоны, мг/л, по ГОСТ 12.1.005-88; К=5 - для раздражающих ядов (по-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>мечены одной звездочкой); К=9 - для всех прочих ядов (помечены двумя звездочками).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">4. Значения </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>K</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>для изотермического хранения аммиака приведены для случая разлива (выброса) в поддон.</t>
-    </r>
-  </si>
-  <si>
     <t>1 1</t>
   </si>
   <si>
     <t>0 0,9</t>
+  </si>
+  <si>
+    <t>06 1</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Соляная кислота (концентрированная) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>(HCI)</t>
+    </r>
+  </si>
+  <si>
+    <t>Аммиак хранение под давлением (NH3)</t>
+  </si>
+  <si>
+    <t>Аммиак изотермическое хранение (NH3)</t>
+  </si>
+  <si>
+    <t>0,02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3898,11 +3394,6 @@
     </font>
     <font>
       <i/>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
       <vertAlign val="subscript"/>
       <sz val="11"/>
       <name val="Times New Roman"/>
@@ -3933,6 +3424,16 @@
       <sz val="7"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3942,7 +3443,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -4325,100 +3826,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -4448,76 +3860,79 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4820,1665 +4235,1502 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7"/>
-    <col min="2" max="2" width="33"/>
-    <col min="3" max="3" width="14"/>
-    <col min="4" max="4" width="15"/>
-    <col min="5" max="6" width="21"/>
-    <col min="7" max="9" width="9"/>
-    <col min="10" max="13" width="7"/>
-    <col min="14" max="14" width="8"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14"/>
+    <col min="3" max="3" width="15"/>
+    <col min="4" max="4" width="21"/>
+    <col min="5" max="5" width="21" style="33"/>
+    <col min="6" max="8" width="9"/>
+    <col min="9" max="12" width="7"/>
+    <col min="13" max="13" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="M2" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="D6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="G6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>133</v>
+      <c r="L6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="K5" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="17" t="s">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>43</v>
+      <c r="D7" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="M7" s="18" t="s">
+      <c r="I8" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N7" s="18" t="s">
-        <v>137</v>
+      <c r="F9" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="M8" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N8" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="17" t="s">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>46</v>
+      <c r="D10" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M27" s="17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="L10" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>138</v>
+      <c r="F29" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" s="14" t="s">
+        <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="8" t="s">
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="L32" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="M32" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="L33" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="M33" s="21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="H34" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N11" s="15" t="s">
-        <v>138</v>
+      <c r="I34" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="J34" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="K34" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="L34" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="M34" s="23" t="s">
+        <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>139</v>
+    <row r="35" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="K35" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="M35" s="23" t="s">
+        <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="L13" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="23" t="s">
+    <row r="36" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="L14" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N14" s="15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="L15" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="L16" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L18" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M18" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" s="18" t="s">
+      <c r="D36" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="H36" s="19" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="L19" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="M19" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N19" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="J20" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L20" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N20" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I22" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="L22" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="M22" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N22" s="15" t="s">
+      <c r="I36" s="19" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="L23" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="M23" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N23" s="15" t="s">
+      <c r="J36" s="23" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="L24" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="M24" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N24" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="L26" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="K27" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="L27" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="M27" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N27" s="15" t="s">
+      <c r="K36" s="23" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="H28" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="L28" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="M28" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N28" s="15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="L29" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="M29" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N29" s="24" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="H30" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="L30" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="M30" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N30" s="15" t="s">
+      <c r="L36" s="23" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H31" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="K31" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L31" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M31" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N31" s="18" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H32" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="J32" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="K32" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="L32" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="M32" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="K33" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="L33" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="M33" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N33" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="I34" s="23" t="s">
-        <v>253</v>
-      </c>
-      <c r="J34" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="K34" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="L34" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="M34" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N34" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>274</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="H36" s="25" t="s">
-        <v>289</v>
-      </c>
-      <c r="I36" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="J36" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="K36" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="L36" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="M36" s="27" t="s">
-        <v>303</v>
-      </c>
-      <c r="N36" s="28" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+      <c r="M36" s="23" t="s">
         <v>271</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H37" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="I37" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="J37" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="K37" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="L37" s="30" t="s">
-        <v>301</v>
-      </c>
-      <c r="M37" s="30" t="s">
-        <v>304</v>
-      </c>
-      <c r="N37" s="30" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="I38" s="30" t="s">
-        <v>294</v>
-      </c>
-      <c r="J38" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="K38" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="L38" s="30" t="s">
-        <v>301</v>
-      </c>
-      <c r="M38" s="30" t="s">
-        <v>304</v>
-      </c>
-      <c r="N38" s="30" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="F39" s="27" t="s">
-        <v>287</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H39" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="I39" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="J39" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>299</v>
-      </c>
-      <c r="L39" s="30" t="s">
-        <v>302</v>
-      </c>
-      <c r="M39" s="30" t="s">
-        <v>304</v>
-      </c>
-      <c r="N39" s="30" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="31" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="31" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="31" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="31" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="31" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="32" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="31" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="31" t="s">
-        <v>315</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>